<commit_message>
Adding latest work to Excel file
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>Array Size</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Linear Time</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -189,6 +192,57 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37513123359580053"/>
+                  <c:y val="-8.3750000000000005E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Enumeration!$A$3:$A$12</c:f>
@@ -235,34 +289,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.2966170310974102E-2</c:v>
+                  <c:v>2.2116923332214301E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16496615409851001</c:v>
+                  <c:v>0.164214706420898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53462767601013095</c:v>
+                  <c:v>0.53818001747131305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84574737548828105</c:v>
+                  <c:v>0.81447532176971404</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.26119110584259</c:v>
+                  <c:v>1.2266164302825899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.77335283756256</c:v>
+                  <c:v>1.72226679325103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.36016845703125</c:v>
+                  <c:v>2.3528623104095399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1408703804016098</c:v>
+                  <c:v>3.1338655710220298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1628911256790104</c:v>
+                  <c:v>4.0759297609329197</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4401938199996902</c:v>
+                  <c:v>5.1409328937530496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,11 +331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1833492448"/>
-        <c:axId val="-1839423056"/>
+        <c:axId val="-1052088192"/>
+        <c:axId val="-1052090912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1833492448"/>
+        <c:axId val="-1052088192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,12 +420,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1839423056"/>
+        <c:crossAx val="-1052090912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1839423056"/>
+        <c:axId val="-1052090912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,7 +524,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1833492448"/>
+        <c:crossAx val="-1052088192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -628,6 +682,57 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.42986220472440945"/>
+                  <c:y val="-6.0535870516185475E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Better Enum'!$A$3:$A$12</c:f>
@@ -674,34 +779,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.5027008056640603E-4</c:v>
+                  <c:v>5.5043697357177698E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2015571594238199E-3</c:v>
+                  <c:v>1.95133686065673E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5537939071655202E-3</c:v>
+                  <c:v>4.7532796859741204E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.20889377593994E-3</c:v>
+                  <c:v>8.9063405990600503E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.50584936141967E-2</c:v>
+                  <c:v>1.4458656311035101E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9290575981140098E-2</c:v>
+                  <c:v>5.67424774169921E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.249278879165649</c:v>
+                  <c:v>0.227708220481872</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98109185695648105</c:v>
+                  <c:v>0.91389586925506505</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.98956956863403</c:v>
+                  <c:v>3.6655384778976399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1392386436462401</c:v>
+                  <c:v>5.7152891635894703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -716,11 +821,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-69292880"/>
-        <c:axId val="-69295056"/>
+        <c:axId val="-1052096352"/>
+        <c:axId val="-1052092544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-69292880"/>
+        <c:axId val="-1052096352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,12 +910,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-69295056"/>
+        <c:crossAx val="-1052092544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-69295056"/>
+        <c:axId val="-1052092544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-69292880"/>
+        <c:crossAx val="-1052096352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1067,6 +1172,57 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.37858661417322836"/>
+                  <c:y val="-8.8526538349373018E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Div and Conq'!$A$3:$A$12</c:f>
@@ -1113,34 +1269,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.0502033233642502E-4</c:v>
+                  <c:v>8.0041885375976504E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5548458099365198E-3</c:v>
+                  <c:v>2.6518583297729399E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0089588165283198E-3</c:v>
+                  <c:v>5.6051969528198202E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9143028259277306E-3</c:v>
+                  <c:v>9.6606254577636698E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6114854812621999E-2</c:v>
+                  <c:v>1.57110452651977E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.19462728500366E-2</c:v>
+                  <c:v>6.1543655395507803E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.244376039505004</c:v>
+                  <c:v>0.245573687553405</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99770812988281199</c:v>
+                  <c:v>0.97238428592681803</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1921643495559602</c:v>
+                  <c:v>3.88760018348693</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4130308151245101</c:v>
+                  <c:v>6.0535747289657502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,11 +1311,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2012273312"/>
-        <c:axId val="-2012274400"/>
+        <c:axId val="-1052088736"/>
+        <c:axId val="-1052087648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2012273312"/>
+        <c:axId val="-1052088736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,12 +1400,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2012274400"/>
+        <c:crossAx val="-1052087648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2012274400"/>
+        <c:axId val="-1052087648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2012273312"/>
+        <c:crossAx val="-1052088736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1506,6 +1662,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.41382152230971131"/>
+                  <c:y val="-5.1342592592592592E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Linear!$A$3:$A$12</c:f>
@@ -1513,34 +1719,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2000</c:v>
+                  <c:v>64000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4000</c:v>
+                  <c:v>128000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8000</c:v>
+                  <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
+                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,34 +1758,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>4.9972534179687499E-5</c:v>
+                  <c:v>3.5011768341064399E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.50156021118164E-4</c:v>
+                  <c:v>6.0048103332519497E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4998188018798801E-4</c:v>
+                  <c:v>1.40078067779541E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0029544830322201E-4</c:v>
+                  <c:v>2.5029659271240201E-3</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>4.9996376037597599E-5</c:v>
+                  <c:v>5.1036596298217702E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9996166229247999E-4</c:v>
+                  <c:v>9.9093914031982405E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5050125122070304E-4</c:v>
+                  <c:v>2.01166868209838E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25064849853515E-3</c:v>
+                  <c:v>4.01779890060424E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.05235385894775E-3</c:v>
+                  <c:v>8.1155800819396898E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1020879745483399E-3</c:v>
+                  <c:v>0.163213491439819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1594,11 +1800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1833493536"/>
-        <c:axId val="-1833488640"/>
+        <c:axId val="-1052086560"/>
+        <c:axId val="-1052085472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1833493536"/>
+        <c:axId val="-1052086560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,12 +1889,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1833488640"/>
+        <c:crossAx val="-1052085472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1833488640"/>
+        <c:axId val="-1052085472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1956,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1787,7 +1993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1833493536"/>
+        <c:crossAx val="-1052086560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4504,7 +4710,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4534,7 +4740,7 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>2.2966170310974102E-2</v>
+        <v>2.2116923332214301E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4542,7 +4748,7 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>0.16496615409851001</v>
+        <v>0.164214706420898</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4550,7 +4756,7 @@
         <v>300</v>
       </c>
       <c r="B5">
-        <v>0.53462767601013095</v>
+        <v>0.53818001747131305</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4558,7 +4764,7 @@
         <v>350</v>
       </c>
       <c r="B6">
-        <v>0.84574737548828105</v>
+        <v>0.81447532176971404</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4566,7 +4772,7 @@
         <v>400</v>
       </c>
       <c r="B7">
-        <v>1.26119110584259</v>
+        <v>1.2266164302825899</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4574,7 +4780,7 @@
         <v>450</v>
       </c>
       <c r="B8">
-        <v>1.77335283756256</v>
+        <v>1.72226679325103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4582,7 +4788,7 @@
         <v>500</v>
       </c>
       <c r="B9">
-        <v>2.36016845703125</v>
+        <v>2.3528623104095399</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4590,7 +4796,7 @@
         <v>550</v>
       </c>
       <c r="B10">
-        <v>3.1408703804016098</v>
+        <v>3.1338655710220298</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4598,7 +4804,7 @@
         <v>600</v>
       </c>
       <c r="B11">
-        <v>4.1628911256790104</v>
+        <v>4.0759297609329197</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -4606,7 +4812,7 @@
         <v>650</v>
       </c>
       <c r="B12">
-        <v>5.4401938199996902</v>
+        <v>5.1409328937530496</v>
       </c>
     </row>
   </sheetData>
@@ -4617,10 +4823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4650,7 +4856,7 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>5.5027008056640603E-4</v>
+        <v>5.5043697357177698E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4658,7 +4864,7 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>2.2015571594238199E-3</v>
+        <v>1.95133686065673E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4666,7 +4872,7 @@
         <v>300</v>
       </c>
       <c r="B5">
-        <v>5.5537939071655202E-3</v>
+        <v>4.7532796859741204E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4674,7 +4880,7 @@
         <v>400</v>
       </c>
       <c r="B6">
-        <v>9.20889377593994E-3</v>
+        <v>8.9063405990600503E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4682,7 +4888,7 @@
         <v>500</v>
       </c>
       <c r="B7">
-        <v>1.50584936141967E-2</v>
+        <v>1.4458656311035101E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4690,7 +4896,7 @@
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>5.9290575981140098E-2</v>
+        <v>5.67424774169921E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4698,7 +4904,7 @@
         <v>2000</v>
       </c>
       <c r="B9">
-        <v>0.249278879165649</v>
+        <v>0.227708220481872</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4706,7 +4912,7 @@
         <v>4000</v>
       </c>
       <c r="B10">
-        <v>0.98109185695648105</v>
+        <v>0.91389586925506505</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4714,7 +4920,7 @@
         <v>8000</v>
       </c>
       <c r="B11">
-        <v>3.98956956863403</v>
+        <v>3.6655384778976399</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -4722,7 +4928,12 @@
         <v>10000</v>
       </c>
       <c r="B12">
-        <v>6.1392386436462401</v>
+        <v>5.7152891635894703</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4736,7 +4947,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4766,7 +4977,7 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>8.0502033233642502E-4</v>
+        <v>8.0041885375976504E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4774,7 +4985,7 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>2.5548458099365198E-3</v>
+        <v>2.6518583297729399E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4782,7 +4993,7 @@
         <v>300</v>
       </c>
       <c r="B5">
-        <v>6.0089588165283198E-3</v>
+        <v>5.6051969528198202E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4790,7 +5001,7 @@
         <v>400</v>
       </c>
       <c r="B6">
-        <v>9.9143028259277306E-3</v>
+        <v>9.6606254577636698E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4798,7 +5009,7 @@
         <v>500</v>
       </c>
       <c r="B7">
-        <v>1.6114854812621999E-2</v>
+        <v>1.57110452651977E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4806,7 +5017,7 @@
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>6.19462728500366E-2</v>
+        <v>6.1543655395507803E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4814,7 +5025,7 @@
         <v>2000</v>
       </c>
       <c r="B9">
-        <v>0.244376039505004</v>
+        <v>0.245573687553405</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4822,7 +5033,7 @@
         <v>4000</v>
       </c>
       <c r="B10">
-        <v>0.99770812988281199</v>
+        <v>0.97238428592681803</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4830,7 +5041,7 @@
         <v>8000</v>
       </c>
       <c r="B11">
-        <v>4.1921643495559602</v>
+        <v>3.88760018348693</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -4838,7 +5049,7 @@
         <v>10000</v>
       </c>
       <c r="B12">
-        <v>6.4130308151245101</v>
+        <v>6.0535747289657502</v>
       </c>
     </row>
   </sheetData>
@@ -4852,7 +5063,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4879,82 +5090,82 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="B3" s="2">
-        <v>4.9972534179687499E-5</v>
+        <v>3.5011768341064399E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="B4">
-        <v>1.50156021118164E-4</v>
+        <v>6.0048103332519497E-4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>300</v>
+        <v>4000</v>
       </c>
       <c r="B5">
-        <v>2.4998188018798801E-4</v>
+        <v>1.40078067779541E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>400</v>
+        <v>8000</v>
       </c>
       <c r="B6">
-        <v>2.0029544830322201E-4</v>
+        <v>2.5029659271240201E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>500</v>
+        <v>16000</v>
       </c>
       <c r="B7" s="2">
-        <v>4.9996376037597599E-5</v>
+        <v>5.1036596298217702E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1000</v>
+        <v>32000</v>
       </c>
       <c r="B8">
-        <v>1.9996166229247999E-4</v>
+        <v>9.9093914031982405E-3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2000</v>
+        <v>64000</v>
       </c>
       <c r="B9">
-        <v>6.5050125122070304E-4</v>
+        <v>2.01166868209838E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4000</v>
+        <v>128000</v>
       </c>
       <c r="B10">
-        <v>1.25064849853515E-3</v>
+        <v>4.01779890060424E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>8000</v>
+        <v>256000</v>
       </c>
       <c r="B11">
-        <v>3.05235385894775E-3</v>
+        <v>8.1155800819396898E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10000</v>
+        <v>512000</v>
       </c>
       <c r="B12">
-        <v>3.1020879745483399E-3</v>
+        <v>0.163213491439819</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed algo 1 and algo 2 to the power trendline
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -202,8 +202,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -331,11 +330,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1052088192"/>
-        <c:axId val="-1052090912"/>
+        <c:axId val="-688488816"/>
+        <c:axId val="-688495888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1052088192"/>
+        <c:axId val="-688488816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,12 +419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052090912"/>
+        <c:crossAx val="-688495888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1052090912"/>
+        <c:axId val="-688495888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052088192"/>
+        <c:crossAx val="-688488816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -692,8 +691,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -821,11 +819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1052096352"/>
-        <c:axId val="-1052092544"/>
+        <c:axId val="-688487728"/>
+        <c:axId val="-688496432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1052096352"/>
+        <c:axId val="-688487728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,12 +908,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052092544"/>
+        <c:crossAx val="-688496432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1052092544"/>
+        <c:axId val="-688496432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052096352"/>
+        <c:crossAx val="-688487728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1311,11 +1309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1052088736"/>
-        <c:axId val="-1052087648"/>
+        <c:axId val="-688493712"/>
+        <c:axId val="-688482832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1052088736"/>
+        <c:axId val="-688493712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,12 +1398,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052087648"/>
+        <c:crossAx val="-688482832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1052087648"/>
+        <c:axId val="-688482832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052088736"/>
+        <c:crossAx val="-688493712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1600,7 +1598,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1800,11 +1797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1052086560"/>
-        <c:axId val="-1052085472"/>
+        <c:axId val="-688497520"/>
+        <c:axId val="-688485008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1052086560"/>
+        <c:axId val="-688497520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1822,7 +1819,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1889,12 +1885,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052085472"/>
+        <c:crossAx val="-688485008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1052085472"/>
+        <c:axId val="-688485008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,7 +1922,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1993,7 +1988,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052086560"/>
+        <c:crossAx val="-688497520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2007,7 +2002,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4710,7 +4704,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4947,7 +4941,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added: Use the regression model to determine the largest input for the algorithm that can be solved in 10 seconds, 30 seconds and 1minute.
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21348" windowHeight="12612"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21348" windowHeight="12612" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enumeration" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Array Size</t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>10 seconds</t>
+  </si>
+  <si>
+    <t>30 seconds</t>
+  </si>
+  <si>
+    <t>60 seconds</t>
+  </si>
+  <si>
+    <t>Largest Input that can be solved for a certain time based on the equation found above</t>
+  </si>
+  <si>
+    <t>3.33337×10^7</t>
+  </si>
+  <si>
+    <t>1×10^8</t>
+  </si>
+  <si>
+    <t>2.×10^8</t>
   </si>
 </sst>
 </file>
@@ -1598,6 +1619,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1819,6 +1841,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1922,6 +1945,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2002,6 +2026,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4701,10 +4726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4809,6 +4834,35 @@
         <v>5.1409328937530496</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>1599</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4817,10 +4871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4925,9 +4979,36 @@
         <v>5.7152891635894703</v>
       </c>
     </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L18" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>12889</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>22206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>31299</v>
       </c>
     </row>
   </sheetData>
@@ -4938,10 +5019,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5046,6 +5127,35 @@
         <v>6.0535747289657502</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>12885</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>22336</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>31598</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5054,16 +5164,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -5162,10 +5273,36 @@
         <v>0.163213491439819</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot of all done
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21348" windowHeight="12612"/>
   </bookViews>
   <sheets>
-    <sheet name="Enumeration" sheetId="1" r:id="rId1"/>
-    <sheet name="Better Enum" sheetId="2" r:id="rId2"/>
-    <sheet name="Div and Conq" sheetId="3" r:id="rId3"/>
-    <sheet name="Linear" sheetId="4" r:id="rId4"/>
+    <sheet name="Chart1" sheetId="6" r:id="rId1"/>
+    <sheet name="Enumeration" sheetId="1" r:id="rId2"/>
+    <sheet name="Better Enum" sheetId="2" r:id="rId3"/>
+    <sheet name="Div and Conq" sheetId="3" r:id="rId4"/>
+    <sheet name="Linear" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -151,6 +152,785 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>All (log plot)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Enumeration!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enumeration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Enumeration!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Enumeration!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.2116923332214301E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.164214706420898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53818001747131305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81447532176971404</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2266164302825899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.72226679325103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3528623104095399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1338655710220298</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0759297609329197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1409328937530496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Better Enum'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Better Enumeration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Better Enum'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Better Enum'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.5043697357177698E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.95133686065673E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7532796859741204E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9063405990600503E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4458656311035101E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.67424774169921E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.227708220481872</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91389586925506505</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6655384778976399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7152891635894703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Div and Conq'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Divide and Conquer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Div and Conq'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Div and Conq'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.0041885375976504E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6518583297729399E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6051969528198202E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6606254577636698E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.57110452651977E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1543655395507803E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.245573687553405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97238428592681803</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.88760018348693</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0535747289657502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Linear!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Linear!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>3.5011768341064399E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0048103332519497E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.40078067779541E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5029659271240201E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>5.1036596298217702E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9093914031982405E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.01166868209838E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.01779890060424E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1155800819396898E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.163213491439819</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="663148432"/>
+        <c:axId val="663168560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="663148432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Enumeration!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Array Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="663168560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="663168560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Enumeration!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="663148432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -351,11 +1131,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="578864864"/>
-        <c:axId val="578855072"/>
+        <c:axId val="814196272"/>
+        <c:axId val="814198448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578864864"/>
+        <c:axId val="814196272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,12 +1220,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578855072"/>
+        <c:crossAx val="814198448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="578855072"/>
+        <c:axId val="814198448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,527 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578864864"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Enumeration (log</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> plot)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Enumeration!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Enumeration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.37513123359580053"/>
-                  <c:y val="-8.3750000000000005E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Enumeration!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>650</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Enumeration!$B$3:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.2116923332214301E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.164214706420898</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.53818001747131305</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.81447532176971404</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2266164302825899</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.72226679325103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.3528623104095399</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.1338655710220298</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.0759297609329197</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.1409328937530496</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="688740368"/>
-        <c:axId val="688728400"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="688740368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>Enumeration!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Array Size</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="688728400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="688728400"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>Enumeration!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Running Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="688740368"/>
+        <c:crossAx val="814196272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1160,6 +1420,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Enumeration (log</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> plot)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1201,11 +1491,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Better Enum'!$B$1</c:f>
+              <c:f>Enumeration!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Better Enumeration</c:v>
+                  <c:v>Enumeration</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1238,8 +1528,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.42986220472440945"/>
-                  <c:y val="-6.0535870516185475E-2"/>
+                  <c:x val="0.37513123359580053"/>
+                  <c:y val="-8.3750000000000005E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1274,7 +1564,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Better Enum'!$A$3:$A$12</c:f>
+              <c:f>Enumeration!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1288,64 +1578,64 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2000</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>4000</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8000</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Better Enum'!$B$3:$B$12</c:f>
+              <c:f>Enumeration!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.5043697357177698E-4</c:v>
+                  <c:v>2.2116923332214301E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.95133686065673E-3</c:v>
+                  <c:v>0.164214706420898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.7532796859741204E-3</c:v>
+                  <c:v>0.53818001747131305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9063405990600503E-3</c:v>
+                  <c:v>0.81447532176971404</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4458656311035101E-2</c:v>
+                  <c:v>1.2266164302825899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.67424774169921E-2</c:v>
+                  <c:v>1.72226679325103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.227708220481872</c:v>
+                  <c:v>2.3528623104095399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.91389586925506505</c:v>
+                  <c:v>3.1338655710220298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6655384778976399</c:v>
+                  <c:v>4.0759297609329197</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7152891635894703</c:v>
+                  <c:v>5.1409328937530496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,11 +1650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="578865952"/>
-        <c:axId val="578866496"/>
+        <c:axId val="814196816"/>
+        <c:axId val="814197360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578865952"/>
+        <c:axId val="814196816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1663,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Better Enum'!$A$2</c:f>
+              <c:f>Enumeration!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1449,13 +1739,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578866496"/>
+        <c:crossAx val="814197360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="578866496"/>
+        <c:axId val="814197360"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1477,7 +1768,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Better Enum'!$B$2</c:f>
+              <c:f>Enumeration!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1553,7 +1844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578865952"/>
+        <c:crossAx val="814196816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1649,31 +1940,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Better Enumeration (log plot)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1874,11 +2140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413235600"/>
-        <c:axId val="413230160"/>
+        <c:axId val="814197904"/>
+        <c:axId val="814201168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413235600"/>
+        <c:axId val="814197904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,14 +2229,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413230160"/>
+        <c:crossAx val="814201168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413230160"/>
+        <c:axId val="814201168"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2068,7 +2333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413235600"/>
+        <c:crossAx val="814197904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2164,6 +2429,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Better Enumeration (log plot)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2205,11 +2495,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Div and Conq'!$B$1</c:f>
+              <c:f>'Better Enum'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Divide and Conquer</c:v>
+                  <c:v>Better Enumeration</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2236,15 +2526,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.37858661417322836"/>
-                  <c:y val="-8.8526538349373018E-2"/>
+                  <c:x val="0.42986220472440945"/>
+                  <c:y val="-6.0535870516185475E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2279,7 +2568,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Div and Conq'!$A$3:$A$12</c:f>
+              <c:f>'Better Enum'!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2318,39 +2607,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Div and Conq'!$B$3:$B$12</c:f>
+              <c:f>'Better Enum'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.0041885375976504E-4</c:v>
+                  <c:v>5.5043697357177698E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6518583297729399E-3</c:v>
+                  <c:v>1.95133686065673E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6051969528198202E-3</c:v>
+                  <c:v>4.7532796859741204E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6606254577636698E-3</c:v>
+                  <c:v>8.9063405990600503E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.57110452651977E-2</c:v>
+                  <c:v>1.4458656311035101E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1543655395507803E-2</c:v>
+                  <c:v>5.67424774169921E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.245573687553405</c:v>
+                  <c:v>0.227708220481872</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97238428592681803</c:v>
+                  <c:v>0.91389586925506505</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.88760018348693</c:v>
+                  <c:v>3.6655384778976399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0535747289657502</c:v>
+                  <c:v>5.7152891635894703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2365,11 +2654,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="578856160"/>
-        <c:axId val="578853984"/>
+        <c:axId val="814207696"/>
+        <c:axId val="814206608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578856160"/>
+        <c:axId val="814207696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,7 +2667,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Div and Conq'!$A$2</c:f>
+              <c:f>'Better Enum'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2454,13 +2743,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578853984"/>
+        <c:crossAx val="814206608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="578853984"/>
+        <c:axId val="814206608"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2482,7 +2772,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Div and Conq'!$B$2</c:f>
+              <c:f>'Better Enum'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2558,7 +2848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578856160"/>
+        <c:crossAx val="814207696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2654,31 +2944,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Divide and Conquer (log plot)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2880,11 +3145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="413231792"/>
-        <c:axId val="413235056"/>
+        <c:axId val="814209328"/>
+        <c:axId val="814210416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="413231792"/>
+        <c:axId val="814209328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2969,14 +3234,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413235056"/>
+        <c:crossAx val="814210416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="413235056"/>
+        <c:axId val="814210416"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3074,7 +3338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413231792"/>
+        <c:crossAx val="814209328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3170,6 +3434,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Divide and Conquer (log plot)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3211,11 +3500,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Linear!$B$1</c:f>
+              <c:f>'Div and Conq'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Linear Time</c:v>
+                  <c:v>Divide and Conquer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3242,14 +3531,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.41382152230971131"/>
-                  <c:y val="-5.1342592592592592E-2"/>
+                  <c:x val="0.37858661417322836"/>
+                  <c:y val="-8.8526538349373018E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3284,78 +3574,78 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Linear!$A$3:$A$12</c:f>
+              <c:f>'Div and Conq'!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>8000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Linear!$B$3:$B$12</c:f>
+              <c:f>'Div and Conq'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>3.5011768341064399E-4</c:v>
+                <c:pt idx="0">
+                  <c:v>8.0041885375976504E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0048103332519497E-4</c:v>
+                  <c:v>2.6518583297729399E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.40078067779541E-3</c:v>
+                  <c:v>5.6051969528198202E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5029659271240201E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.1036596298217702E-3</c:v>
+                  <c:v>9.6606254577636698E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.57110452651977E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9093914031982405E-3</c:v>
+                  <c:v>6.1543655395507803E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.01166868209838E-2</c:v>
+                  <c:v>0.245573687553405</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.01779890060424E-2</c:v>
+                  <c:v>0.97238428592681803</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.1155800819396898E-2</c:v>
+                  <c:v>3.88760018348693</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.163213491439819</c:v>
+                  <c:v>6.0535747289657502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3370,11 +3660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="578868128"/>
-        <c:axId val="578854528"/>
+        <c:axId val="698700944"/>
+        <c:axId val="817149056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578868128"/>
+        <c:axId val="698700944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,7 +3673,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>Linear!$A$2</c:f>
+              <c:f>'Div and Conq'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3459,13 +3749,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578854528"/>
+        <c:crossAx val="817149056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="578854528"/>
+        <c:axId val="817149056"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3487,7 +3778,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>Linear!$B$2</c:f>
+              <c:f>'Div and Conq'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3526,7 +3817,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3563,7 +3854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578868128"/>
+        <c:crossAx val="698700944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3659,31 +3950,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Linear Time (log plot)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3884,11 +4150,525 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="582892256"/>
-        <c:axId val="582887904"/>
+        <c:axId val="817151232"/>
+        <c:axId val="817139264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="582892256"/>
+        <c:axId val="817151232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Array Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="817139264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="817139264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="817151232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Linear Time (log plot)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.41382152230971131"/>
+                  <c:y val="-5.1342592592592592E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Linear!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Linear!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>3.5011768341064399E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0048103332519497E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.40078067779541E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5029659271240201E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>5.1036596298217702E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9093914031982405E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.01166868209838E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.01779890060424E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1155800819396898E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.163213491439819</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="817142528"/>
+        <c:axId val="817151776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="817142528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3973,12 +4753,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="582887904"/>
+        <c:crossAx val="817151776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="582887904"/>
+        <c:axId val="817151776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4078,7 +4858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="582892256"/>
+        <c:crossAx val="817142528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4479,6 +5259,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8607,7 +9427,561 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8650574" cy="6277131"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8674,7 +10048,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8743,7 +10117,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8812,7 +10186,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9146,8 +10520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>